<commit_message>
[1723 hvnl] AI Ut-Amf
</commit_message>
<xml_diff>
--- a/hvnl-8687.xlsx
+++ b/hvnl-8687.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8622F6-8398-4C46-8E3A-78C10AF739B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7723F238-25CA-447B-9A77-AC31AAE7B13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3218" windowWidth="15248" windowHeight="11647" xr2:uid="{71459310-C0CE-4645-A29E-CDA61D813831}"/>
+    <workbookView xWindow="1365" yWindow="2138" windowWidth="15247" windowHeight="11647" xr2:uid="{71459310-C0CE-4645-A29E-CDA61D813831}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Naam</t>
   </si>
@@ -88,16 +88,6 @@
 08:07 Amf
 08:12 Amf
 08:37 Apd</t>
-  </si>
-  <si>
-    <t>Ut 07:38-07:57
-Tabel 20a: incompleet
-Tabel 20b:
-[n] 6018 &gt;?
-[x] 1818
-[x] 7318 &lt;?
-[x] 9618 &gt;?
-[n] 9620(A) &gt;?</t>
   </si>
   <si>
     <t>Tabel 21a:
@@ -161,6 +151,98 @@
 [x] 1718
 [x] 3618 &gt;?
 [x] 5620 &gt;?</t>
+  </si>
+  <si>
+    <t>Tabel 34a:
+[x] 3623
+[x] 5623
+Tabel 34b:
+[x] 3618
+[x] 5620/7420</t>
+  </si>
+  <si>
+    <t>Tabel 80a:
+[x] 3623
+[x] 5623
+Tabel 80b:
+[x] 3618
+[x] 5620 (1)
+[x] 7420
+[x] 520
+[x] 3620</t>
+  </si>
+  <si>
+    <t>Tabel 70a:
+[x] 3623
+[x] 5623
+Tabel 70b:
+[x] 3618
+[x] 5620
+[x] 5620/7420
+[x] 520
+[x] 3620</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ut-Amf 07:52-08:07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Tabel 32a:
+[n] 3921
+[n] 5723
+Tabel 32b:
+[x] 5720
+[n] 3922</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ut 07:38-07:57</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Tabel 20a: incompleet
+Tabel 20b:
+[n] 6018 &gt;?
+[x] 1818
+[x] 7318 &lt;?
+[x] 9618 &gt;?
+[n] 9620(A) &gt;?</t>
+    </r>
+  </si>
+  <si>
+    <t>Amf 08:02-08:17</t>
   </si>
 </sst>
 </file>
@@ -538,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DD2AF9-E550-4C43-AE07-4179A9D54E7F}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -577,104 +659,136 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="114" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B12" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B14" s="3"/>
+    <row r="14" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" s="1" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[1723 hvnl] AI Amf-Apd
</commit_message>
<xml_diff>
--- a/hvnl-8687.xlsx
+++ b/hvnl-8687.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7723F238-25CA-447B-9A77-AC31AAE7B13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86960977-B462-4C9D-9B7E-A3ED063ECF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="2138" windowWidth="15247" windowHeight="11647" xr2:uid="{71459310-C0CE-4645-A29E-CDA61D813831}"/>
+    <workbookView xWindow="-3832" yWindow="570" windowWidth="15247" windowHeight="11648" xr2:uid="{71459310-C0CE-4645-A29E-CDA61D813831}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Naam</t>
   </si>
@@ -151,6 +151,10 @@
 [x] 1718
 [x] 3618 &gt;?
 [x] 5620 &gt;?</t>
+  </si>
+  <si>
+    <t>Tabel 70a:
+Tabel 70b:</t>
   </si>
   <si>
     <t>Tabel 34a:
@@ -242,7 +246,114 @@
     </r>
   </si>
   <si>
-    <t>Amf 08:02-08:17</t>
+    <t>Tabel 71a:
+Tabel 71b:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Amf 08:02-08:17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Tabel 35a:
+Tabel 35b:
+[x] 7422 &gt;?</t>
+    </r>
+  </si>
+  <si>
+    <t>Tabel 80a:
+[x] 3623
+[x] 723 &lt;?
+[x] 5623
+Tabel 80b:
+[x] D1244 &lt;?
+[x] 5622</t>
+  </si>
+  <si>
+    <t>Tabel 70a:
+[x] 5623
+Tabel 70b:
+[x] D1244 TODO
+[x] 5622 &lt;?</t>
+  </si>
+  <si>
+    <t>Tabel 81a:
+[x] 723
+[x] 5623 &lt;?
+Tabel 81b:
+[x] 5822
+[x] 5622 &gt;?</t>
+  </si>
+  <si>
+    <t>Tabel 71a:
+[n] (D)2241
+[x] 723 &gt;?
+Tabel 71b:
+[x] 5822 &lt;?
+[x] D1244 &gt;?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Amf-Apd 08:12-08:37</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Tabel 35a:
+Tabel 35b:
+[x] 7422 &gt;7423
+[x] 7424 &gt;7425</t>
+    </r>
+  </si>
+  <si>
+    <t>Tabel 70a:
+Tabel 70b:
+[x] 1722
+[x] 1624</t>
+  </si>
+  <si>
+    <t>Tabel 71a:
+Tabel 71b:
+[x] 1722
+[x] 1624</t>
+  </si>
+  <si>
+    <t>Apd 08:32-08:42
+Tabel 61a:
+Tabel 61b:</t>
+  </si>
+  <si>
+    <t>Tabel 63a:
+Tabel 63b:</t>
   </si>
 </sst>
 </file>
@@ -266,7 +377,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +387,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -304,6 +421,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -620,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DD2AF9-E550-4C43-AE07-4179A9D54E7F}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -659,7 +782,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
@@ -699,91 +822,143 @@
     </row>
     <row r="12" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B16" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="B16" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B18" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B19" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B20" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B21" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B24" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B25" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B27" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B30" s="5"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[1723 hvnl] AI apd
</commit_message>
<xml_diff>
--- a/hvnl-8687.xlsx
+++ b/hvnl-8687.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86960977-B462-4C9D-9B7E-A3ED063ECF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4D28D6-6B48-48C2-85F4-2C0ABF2FC511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3832" yWindow="570" windowWidth="15247" windowHeight="11648" xr2:uid="{71459310-C0CE-4645-A29E-CDA61D813831}"/>
   </bookViews>
@@ -153,10 +153,6 @@
 [x] 5620 &gt;?</t>
   </si>
   <si>
-    <t>Tabel 70a:
-Tabel 70b:</t>
-  </si>
-  <si>
     <t>Tabel 34a:
 [x] 3623
 [x] 5623
@@ -347,13 +343,40 @@
 [x] 1624</t>
   </si>
   <si>
-    <t>Apd 08:32-08:42
+    <t>Tabel 63a:
+[x] 7823
+Tabel 63b:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apd 08:32-08:42</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Tabel 61a:
+[x] 7823 &lt;7824?
 Tabel 61b:</t>
-  </si>
-  <si>
-    <t>Tabel 63a:
-Tabel 63b:</t>
+    </r>
+  </si>
+  <si>
+    <t>Tabel 70a:
+Tabel 70b:
+[x] D236 TODO</t>
   </si>
 </sst>
 </file>
@@ -745,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DD2AF9-E550-4C43-AE07-4179A9D54E7F}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -782,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
@@ -822,82 +845,82 @@
     </row>
     <row r="12" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="57" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="57" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="57" x14ac:dyDescent="0.45">
       <c r="B23" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="B24" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B25" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B24" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B25" s="5" t="s">
+    <row r="26" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B26" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B26" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="27" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B27" s="5" t="s">
-        <v>29</v>
+      <c r="B27" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
[1723 hvnl] script en briefing
</commit_message>
<xml_diff>
--- a/hvnl-8687.xlsx
+++ b/hvnl-8687.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0B508D-5A1D-403E-86CC-D5428B29EDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80A4062-A437-4A9E-A0FB-B56FB413B63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1702" yWindow="2475" windowWidth="15248" windowHeight="11648" xr2:uid="{71459310-C0CE-4645-A29E-CDA61D813831}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Naam</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Altijd-rood</t>
-  </si>
-  <si>
-    <t>Koersborden</t>
   </si>
   <si>
     <t>Scenario script (WX)</t>
@@ -383,6 +380,12 @@
   </si>
   <si>
     <t>Amf</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Koersborden/loknrs</t>
   </si>
 </sst>
 </file>
@@ -762,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DD2AF9-E550-4C43-AE07-4179A9D54E7F}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -778,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -791,7 +794,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="114" x14ac:dyDescent="0.45">
@@ -799,122 +802,122 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="114" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="57" x14ac:dyDescent="0.45">
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="57" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="57" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="57" x14ac:dyDescent="0.45">
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
@@ -934,7 +937,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
@@ -948,7 +951,7 @@
         <v>6</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
@@ -968,7 +971,7 @@
         <v>9</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
@@ -979,17 +982,23 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>